<commit_message>
Fixing Results directory structure. Adding xlsx files for various test.
</commit_message>
<xml_diff>
--- a/SCFrameworkImpl/Results/Charts/2015-03-05.xlsx
+++ b/SCFrameworkImpl/Results/Charts/2015-03-05.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15450" windowHeight="7995" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="15450" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="NumberOfTasks" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="Distribution" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -781,24 +780,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98043008"/>
-        <c:axId val="98044544"/>
+        <c:axId val="54260096"/>
+        <c:axId val="54261632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98043008"/>
+        <c:axId val="54260096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98044544"/>
+        <c:crossAx val="54261632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98044544"/>
+        <c:axId val="54261632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,20 +805,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98043008"/>
+        <c:crossAx val="54260096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1002,24 +1000,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98073984"/>
-        <c:axId val="98092160"/>
+        <c:axId val="76905088"/>
+        <c:axId val="76915072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98073984"/>
+        <c:axId val="76905088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98092160"/>
+        <c:crossAx val="76915072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98092160"/>
+        <c:axId val="76915072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,20 +1025,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98073984"/>
+        <c:crossAx val="76905088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1223,24 +1220,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98105216"/>
-        <c:axId val="98106752"/>
+        <c:axId val="77399168"/>
+        <c:axId val="77400704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98105216"/>
+        <c:axId val="77399168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98106752"/>
+        <c:crossAx val="77400704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98106752"/>
+        <c:axId val="77400704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,20 +1245,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98105216"/>
+        <c:crossAx val="77399168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1388,24 +1384,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101388288"/>
-        <c:axId val="101389824"/>
+        <c:axId val="77544448"/>
+        <c:axId val="77550336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101388288"/>
+        <c:axId val="77544448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101389824"/>
+        <c:crossAx val="77550336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101389824"/>
+        <c:axId val="77550336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,20 +1409,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101388288"/>
+        <c:crossAx val="77544448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1553,24 +1548,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101402496"/>
-        <c:axId val="101404032"/>
+        <c:axId val="77583488"/>
+        <c:axId val="77585024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101402496"/>
+        <c:axId val="77583488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101404032"/>
+        <c:crossAx val="77585024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101404032"/>
+        <c:axId val="77585024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1579,20 +1574,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101402496"/>
+        <c:crossAx val="77583488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1775,24 +1769,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101532416"/>
-        <c:axId val="101533952"/>
+        <c:axId val="87097344"/>
+        <c:axId val="87098880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101532416"/>
+        <c:axId val="87097344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101533952"/>
+        <c:crossAx val="87098880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101533952"/>
+        <c:axId val="87098880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1801,20 +1795,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101532416"/>
+        <c:crossAx val="87097344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1941,24 +1934,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101567104"/>
-        <c:axId val="101572992"/>
+        <c:axId val="87136128"/>
+        <c:axId val="87137664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101567104"/>
+        <c:axId val="87136128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101572992"/>
+        <c:crossAx val="87137664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101572992"/>
+        <c:axId val="87137664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,7 +1959,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101567104"/>
+        <c:crossAx val="87136128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1979,7 +1972,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2106,24 +2099,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="101479168"/>
-        <c:axId val="101480704"/>
+        <c:axId val="87212032"/>
+        <c:axId val="87213568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101479168"/>
+        <c:axId val="87212032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101480704"/>
+        <c:crossAx val="87213568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101480704"/>
+        <c:axId val="87213568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2124,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101479168"/>
+        <c:crossAx val="87212032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2144,7 +2137,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3145,14 +3138,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="1:5">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -3209,7 +3202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>